<commit_message>
adding type of roadTypes about buses
</commit_message>
<xml_diff>
--- a/Estaciones_Troncales_de_TRANSMILENIO.xlsx
+++ b/Estaciones_Troncales_de_TRANSMILENIO.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esmith/Desktop/Files/PersonalProjects/TMSolutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E2F4C8-781E-4247-9C46-557D2E9A70F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00369A84-EA66-1946-90F0-BD1F04A2D9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estaciones_Troncales_de_TRANSMI" sheetId="1" r:id="rId1"/>
     <sheet name="statioType" sheetId="2" r:id="rId2"/>
+    <sheet name="roadBusType" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Estaciones_Troncales_de_TRANSMI!$A$1:$Z$150</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="1367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="1371">
   <si>
     <t>X</t>
   </si>
@@ -4134,14 +4135,214 @@
     <t>SITP</t>
   </si>
   <si>
-    <t>Mixta(M-)</t>
+    <t>Dual(M)</t>
+  </si>
+  <si>
+    <r>
+      <t>INSERT INTO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> [dbo].[tbBusRoadTypes] (roadType) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>VALUES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>'Transmilenio'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INSERT INTO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> [dbo].[tbBusRoadTypes] (roadType) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>VALUES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>'Alimentador'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INSERT INTO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> [dbo].[tbBusRoadTypes] (roadType) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>VALUES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>'SITP'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INSERT INTO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> [dbo].[tbBusRoadTypes] (roadType) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>VALUES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>'Dual(M)'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>);</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4275,6 +4476,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF569CD6"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -4618,9 +4837,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -14249,8 +14469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AEBEED-A487-7A4D-89E6-A483DEA4CCF4}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14279,7 +14499,7 @@
         <v>1364</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D4" si="0">"INSERT INTO [dbo].[tbStationTypes] (stationType) VALUES ('"&amp;B2&amp;"');"</f>
+        <f t="shared" ref="D2:D3" si="0">"INSERT INTO [dbo].[tbStationTypes] (stationType) VALUES ('"&amp;B2&amp;"');"</f>
         <v>INSERT INTO [dbo].[tbStationTypes] (stationType) VALUES ('Alimentador');</v>
       </c>
     </row>
@@ -14304,7 +14524,69 @@
       </c>
       <c r="D4" t="str">
         <f>"INSERT INTO [dbo].[tbStationTypes] (stationType) VALUES ('"&amp;B4&amp;"')"</f>
-        <v>INSERT INTO [dbo].[tbStationTypes] (stationType) VALUES ('Mixta(M-)')</v>
+        <v>INSERT INTO [dbo].[tbStationTypes] (stationType) VALUES ('Dual(M)')</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9EAC718-B457-7F4B-BF45-6479E9148BD9}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>